<commit_message>
Update Presentation und Excel 4
</commit_message>
<xml_diff>
--- a/Presentations/Grafiken_Excel.xlsx
+++ b/Presentations/Grafiken_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Medical_Imaging\Medical_Imaging_Elias\Presentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E52D99A-13F9-4A33-85D3-A4E929864620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768BD1D9-1DC8-4196-B54C-D4B4D7AEEF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="17160" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5F9B5544-9973-4902-BB61-119F88A4B9D5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
   <si>
     <t>Resolution</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Metric</t>
+  </si>
+  <si>
+    <t>Resolution &amp; Pixelsize</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -292,11 +295,161 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,10 +469,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -341,16 +504,91 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -681,27 +919,27 @@
   <sheetData>
     <row r="2" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D5" s="15"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
@@ -779,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639D8EE6-87DA-48EA-95A0-409FDEB618F9}">
-  <dimension ref="D4:Q21"/>
+  <dimension ref="D4:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,159 +1032,159 @@
   <sheetData>
     <row r="4" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="5" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="13"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="17"/>
     </row>
     <row r="6" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="10"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="14"/>
     </row>
     <row r="7" spans="4:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="E7" s="15"/>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="21"/>
+      <c r="F7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="Q7" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="9">
         <v>0.78</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="9">
         <v>0.77</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="9">
         <v>0.79</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="9">
         <v>0.69</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="9">
         <v>0.71</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="9">
         <v>0.75</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="9">
         <v>0.7</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="9">
         <v>0.62</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="9">
         <v>0.73</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="9">
         <v>0.73</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="9">
         <v>0.69</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="9">
         <v>0.69</v>
       </c>
     </row>
-    <row r="9" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="E9" s="8" t="s">
+    <row r="9" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="10">
         <v>0.92</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="10">
         <v>0.9</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="10">
         <v>0.92</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="10">
         <v>0.89</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="10">
         <v>0.88</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="10">
         <v>0.9</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="10">
         <v>0.89</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="10">
         <v>0.83</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="10">
         <v>0.88</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="10">
         <v>0.88</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="10">
         <v>0.87</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="10">
         <v>0.85</v>
       </c>
     </row>
@@ -959,347 +1197,748 @@
     </row>
     <row r="12" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="13"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="26"/>
     </row>
     <row r="14" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="18"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="28"/>
     </row>
     <row r="15" spans="4:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="7" t="s">
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="M15" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="7" t="s">
+      <c r="N15" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="7" t="s">
+      <c r="O15" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P15" s="7" t="s">
+      <c r="P15" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="Q15" s="7" t="s">
+      <c r="Q15" s="29" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="30">
         <v>0.92</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="30">
         <v>0.78</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="30">
         <v>0.93</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="30">
         <v>0.81</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="30">
         <v>0.74</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="30">
         <v>0.82</v>
       </c>
-      <c r="L16" s="19">
+      <c r="L16" s="30">
         <v>0.84</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="30">
         <v>0.62</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="30">
         <v>0.75</v>
       </c>
-      <c r="O16" s="19">
+      <c r="O16" s="30">
         <v>0.78</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="30">
         <v>0.78</v>
       </c>
-      <c r="Q16" s="19">
+      <c r="Q16" s="30">
         <v>0.69</v>
       </c>
     </row>
     <row r="17" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D17" s="17"/>
-      <c r="E17" s="8" t="s">
+      <c r="D17" s="22"/>
+      <c r="E17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="30">
         <v>0.87</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="30">
         <v>0.89</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="30">
         <v>0.88</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="30">
         <v>0.84</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="30">
         <v>0.86</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="30">
         <v>0.87</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="30">
         <v>0.84</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="30">
         <v>0.83</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N17" s="30">
         <v>0.87</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O17" s="30">
         <v>0.86</v>
       </c>
-      <c r="P17" s="19">
+      <c r="P17" s="30">
         <v>0.83</v>
       </c>
-      <c r="Q17" s="19">
+      <c r="Q17" s="30">
         <v>0.85</v>
       </c>
     </row>
     <row r="18" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="30">
         <v>0.67</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="30">
         <v>0.77</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="30">
         <v>0.7</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="30">
         <v>0.6</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="30">
         <v>0.69</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="30">
         <v>0.7</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="30">
         <v>0.6</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="30">
         <v>0.62</v>
       </c>
-      <c r="N18" s="19">
+      <c r="N18" s="30">
         <v>0.71</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="30">
         <v>0.69</v>
       </c>
-      <c r="P18" s="19">
+      <c r="P18" s="30">
         <v>0.62</v>
       </c>
-      <c r="Q18" s="19">
+      <c r="Q18" s="30">
         <v>0.69</v>
       </c>
     </row>
     <row r="19" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D19" s="17"/>
-      <c r="E19" s="8" t="s">
+      <c r="D19" s="22"/>
+      <c r="E19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="30">
         <v>0.97</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="30">
         <v>0.9</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="30">
         <v>0.97</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="30">
         <v>0.94</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="30">
         <v>0.89</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="30">
         <v>0.93</v>
       </c>
-      <c r="L19" s="19">
+      <c r="L19" s="30">
         <v>0.95</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="30">
         <v>0.83</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N19" s="30">
         <v>0.89</v>
       </c>
-      <c r="O19" s="19">
+      <c r="O19" s="30">
         <v>0.91</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="30">
         <v>0.92</v>
       </c>
-      <c r="Q19" s="19">
+      <c r="Q19" s="30">
         <v>0.85</v>
       </c>
     </row>
     <row r="20" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="30">
         <v>0.78</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="30">
         <v>0.77</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="30">
         <v>0.79</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="30">
         <v>0.69</v>
       </c>
-      <c r="J20" s="19">
+      <c r="J20" s="30">
         <v>0.71</v>
       </c>
-      <c r="K20" s="19">
+      <c r="K20" s="30">
         <v>0.75</v>
       </c>
-      <c r="L20" s="19">
+      <c r="L20" s="30">
         <v>0.7</v>
       </c>
-      <c r="M20" s="19">
+      <c r="M20" s="30">
         <v>0.62</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="30">
         <v>0.73</v>
       </c>
-      <c r="O20" s="19">
+      <c r="O20" s="30">
         <v>0.73</v>
       </c>
-      <c r="P20" s="19">
+      <c r="P20" s="30">
         <v>0.69</v>
       </c>
-      <c r="Q20" s="19">
+      <c r="Q20" s="30">
         <v>0.69</v>
       </c>
     </row>
     <row r="21" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="30">
         <v>0.92</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="30">
         <v>0.9</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="30">
         <v>0.92</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="30">
         <v>0.89</v>
       </c>
-      <c r="J21" s="19">
+      <c r="J21" s="30">
         <v>0.88</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="30">
         <v>0.9</v>
       </c>
-      <c r="L21" s="19">
+      <c r="L21" s="30">
         <v>0.89</v>
       </c>
-      <c r="M21" s="19">
+      <c r="M21" s="30">
         <v>0.83</v>
       </c>
-      <c r="N21" s="19">
+      <c r="N21" s="30">
         <v>0.88</v>
       </c>
-      <c r="O21" s="19">
+      <c r="O21" s="30">
         <v>0.88</v>
       </c>
-      <c r="P21" s="19">
+      <c r="P21" s="30">
         <v>0.87</v>
       </c>
-      <c r="Q21" s="19">
+      <c r="Q21" s="30">
         <v>0.85</v>
       </c>
     </row>
+    <row r="22" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+    </row>
+    <row r="23" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+    </row>
+    <row r="24" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D25" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D26" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="34"/>
+      <c r="G26" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="34"/>
+      <c r="I26" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="34"/>
+    </row>
+    <row r="27" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D27" s="35"/>
+      <c r="E27" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="4:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="D28" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="44">
+        <v>0.92</v>
+      </c>
+      <c r="F28" s="45">
+        <v>0.87</v>
+      </c>
+      <c r="G28" s="44">
+        <v>0.67</v>
+      </c>
+      <c r="H28" s="45">
+        <v>0.97</v>
+      </c>
+      <c r="I28" s="44">
+        <v>0.78</v>
+      </c>
+      <c r="J28" s="45">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="29" spans="4:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="D29" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="47">
+        <v>0.78</v>
+      </c>
+      <c r="F29" s="48">
+        <v>0.89</v>
+      </c>
+      <c r="G29" s="47">
+        <v>0.77</v>
+      </c>
+      <c r="H29" s="48">
+        <v>0.9</v>
+      </c>
+      <c r="I29" s="47">
+        <v>0.77</v>
+      </c>
+      <c r="J29" s="48">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="30" spans="4:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="D30" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="47">
+        <v>0.93</v>
+      </c>
+      <c r="F30" s="48">
+        <v>0.88</v>
+      </c>
+      <c r="G30" s="47">
+        <v>0.7</v>
+      </c>
+      <c r="H30" s="48">
+        <v>0.97</v>
+      </c>
+      <c r="I30" s="47">
+        <v>0.79</v>
+      </c>
+      <c r="J30" s="48">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="31" spans="4:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="D31" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="47">
+        <v>0.81</v>
+      </c>
+      <c r="F31" s="48">
+        <v>0.84</v>
+      </c>
+      <c r="G31" s="47">
+        <v>0.6</v>
+      </c>
+      <c r="H31" s="48">
+        <v>0.94</v>
+      </c>
+      <c r="I31" s="47">
+        <v>0.69</v>
+      </c>
+      <c r="J31" s="48">
+        <v>0.89</v>
+      </c>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+    </row>
+    <row r="32" spans="4:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="D32" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="47">
+        <v>0.74</v>
+      </c>
+      <c r="F32" s="48">
+        <v>0.86</v>
+      </c>
+      <c r="G32" s="47">
+        <v>0.69</v>
+      </c>
+      <c r="H32" s="48">
+        <v>0.89</v>
+      </c>
+      <c r="I32" s="47">
+        <v>0.71</v>
+      </c>
+      <c r="J32" s="48">
+        <v>0.88</v>
+      </c>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+    </row>
+    <row r="33" spans="4:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="D33" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="47">
+        <v>0.82</v>
+      </c>
+      <c r="F33" s="48">
+        <v>0.87</v>
+      </c>
+      <c r="G33" s="47">
+        <v>0.7</v>
+      </c>
+      <c r="H33" s="48">
+        <v>0.93</v>
+      </c>
+      <c r="I33" s="47">
+        <v>0.75</v>
+      </c>
+      <c r="J33" s="48">
+        <v>0.9</v>
+      </c>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29"/>
+    </row>
+    <row r="34" spans="4:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="D34" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="47">
+        <v>0.84</v>
+      </c>
+      <c r="F34" s="48">
+        <v>0.84</v>
+      </c>
+      <c r="G34" s="47">
+        <v>0.6</v>
+      </c>
+      <c r="H34" s="48">
+        <v>0.95</v>
+      </c>
+      <c r="I34" s="47">
+        <v>0.7</v>
+      </c>
+      <c r="J34" s="48">
+        <v>0.89</v>
+      </c>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29"/>
+    </row>
+    <row r="35" spans="4:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="D35" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="47">
+        <v>0.62</v>
+      </c>
+      <c r="F35" s="48">
+        <v>0.83</v>
+      </c>
+      <c r="G35" s="47">
+        <v>0.62</v>
+      </c>
+      <c r="H35" s="48">
+        <v>0.83</v>
+      </c>
+      <c r="I35" s="47">
+        <v>0.62</v>
+      </c>
+      <c r="J35" s="48">
+        <v>0.83</v>
+      </c>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="O35" s="29"/>
+    </row>
+    <row r="36" spans="4:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="D36" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="47">
+        <v>0.75</v>
+      </c>
+      <c r="F36" s="48">
+        <v>0.87</v>
+      </c>
+      <c r="G36" s="47">
+        <v>0.71</v>
+      </c>
+      <c r="H36" s="48">
+        <v>0.89</v>
+      </c>
+      <c r="I36" s="47">
+        <v>0.73</v>
+      </c>
+      <c r="J36" s="48">
+        <v>0.88</v>
+      </c>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+    </row>
+    <row r="37" spans="4:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="D37" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="47">
+        <v>0.78</v>
+      </c>
+      <c r="F37" s="48">
+        <v>0.86</v>
+      </c>
+      <c r="G37" s="47">
+        <v>0.69</v>
+      </c>
+      <c r="H37" s="48">
+        <v>0.91</v>
+      </c>
+      <c r="I37" s="47">
+        <v>0.73</v>
+      </c>
+      <c r="J37" s="48">
+        <v>0.88</v>
+      </c>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+    </row>
+    <row r="38" spans="4:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="D38" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="47">
+        <v>0.78</v>
+      </c>
+      <c r="F38" s="48">
+        <v>0.83</v>
+      </c>
+      <c r="G38" s="47">
+        <v>0.62</v>
+      </c>
+      <c r="H38" s="48">
+        <v>0.92</v>
+      </c>
+      <c r="I38" s="47">
+        <v>0.69</v>
+      </c>
+      <c r="J38" s="48">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="39" spans="4:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D39" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="42">
+        <v>0.69</v>
+      </c>
+      <c r="F39" s="40">
+        <v>0.85</v>
+      </c>
+      <c r="G39" s="42">
+        <v>0.69</v>
+      </c>
+      <c r="H39" s="40">
+        <v>0.85</v>
+      </c>
+      <c r="I39" s="42">
+        <v>0.69</v>
+      </c>
+      <c r="J39" s="40">
+        <v>0.85</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D25:J25"/>
+    <mergeCell ref="E5:Q5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:Q6"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="E14:E15"/>
@@ -1307,9 +1946,6 @@
     <mergeCell ref="D13:Q13"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E5:Q5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1384,11 +2020,11 @@
       <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>

</xml_diff>